<commit_message>
Attempting to fix bug where well locations are offset in the final output. In the output lines, the second instance of the well location is incorrect.
</commit_message>
<xml_diff>
--- a/JM1013_worklist_8_22_2025.xlsx
+++ b/JM1013_worklist_8_22_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://byu.sharepoint.com/sites/PROJECTS9/Shared Documents/LCM/Projects+Experiments/JM1013_U of U Mouse Brains/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01c1829094dbd390/Desktop/Kelly_Lab/.venv/worklist_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="151" documentId="8_{8F1F7B8B-A6B8-40F4-9B0E-D7DD1F605021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{712BC300-DCCE-4AD5-9073-152B9BE3AA47}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF50EA0A-2797-EC49-8565-645DB7B38C61}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BF50EA0A-2797-EC49-8565-645DB7B38C61}"/>
   </bookViews>
   <sheets>
     <sheet name="Worklist Generator" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -903,7 +903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,16 +1240,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79332BF3-487A-D048-AE38-CBE359952258}">
   <dimension ref="A1:AP58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="AF27" sqref="AF27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="41" workbookViewId="0">
+      <selection activeCell="AJ36" sqref="AJ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="18.25" customWidth="1"/>
     <col min="3" max="3" width="3.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="4" max="4" width="6.58203125" customWidth="1"/>
     <col min="5" max="28" width="3.25" customWidth="1"/>
     <col min="29" max="29" width="3.25" style="1" customWidth="1"/>
     <col min="30" max="30" width="17.25" customWidth="1"/>
@@ -1267,7 +1267,7 @@
     <col min="42" max="42" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="D4" s="1"/>
@@ -1476,7 +1476,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A6" s="21" t="s">
         <v>36</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.4">
       <c r="B7" s="7"/>
       <c r="D7" t="s">
         <v>40</v>
@@ -1741,7 +1741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D8" t="s">
         <v>42</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
         <v>44</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
         <v>52</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D13" t="s">
         <v>55</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D14" t="s">
         <v>58</v>
       </c>
@@ -2371,7 +2371,7 @@
       <c r="AO14" s="25"/>
       <c r="AP14" s="26"/>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
         <v>59</v>
       </c>
@@ -2415,7 +2415,7 @@
       <c r="AO15" s="25"/>
       <c r="AP15" s="26"/>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D16" t="s">
         <v>60</v>
       </c>
@@ -2459,7 +2459,7 @@
       <c r="AO16" s="25"/>
       <c r="AP16" s="26"/>
     </row>
-    <row r="17" spans="1:42">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D17" t="s">
         <v>61</v>
       </c>
@@ -2503,7 +2503,7 @@
       <c r="AO17" s="25"/>
       <c r="AP17" s="26"/>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D18" t="s">
         <v>62</v>
       </c>
@@ -2547,7 +2547,7 @@
       <c r="AO18" s="25"/>
       <c r="AP18" s="26"/>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D19" t="s">
         <v>63</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="AO19" s="25"/>
       <c r="AP19" s="26"/>
     </row>
-    <row r="20" spans="1:42">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D20" t="s">
         <v>64</v>
       </c>
@@ -2635,7 +2635,7 @@
       <c r="AO20" s="25"/>
       <c r="AP20" s="26"/>
     </row>
-    <row r="21" spans="1:42">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D21" t="s">
         <v>65</v>
       </c>
@@ -2679,7 +2679,7 @@
       <c r="AO21" s="25"/>
       <c r="AP21" s="26"/>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="D22" s="1"/>
@@ -2723,7 +2723,7 @@
       <c r="AO22" s="25"/>
       <c r="AP22" s="26"/>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A23" s="15" t="s">
         <v>32</v>
       </c>
@@ -2821,7 +2821,7 @@
       <c r="AO23" s="25"/>
       <c r="AP23" s="26"/>
     </row>
-    <row r="24" spans="1:42">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A24" s="21" t="s">
         <v>40</v>
       </c>
@@ -2871,7 +2871,7 @@
       <c r="AO24" s="25"/>
       <c r="AP24" s="26"/>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D25" t="s">
         <v>40</v>
       </c>
@@ -2915,7 +2915,7 @@
       <c r="AO25" s="25"/>
       <c r="AP25" s="26"/>
     </row>
-    <row r="26" spans="1:42">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D26" t="s">
         <v>42</v>
       </c>
@@ -2959,7 +2959,7 @@
       <c r="AO26" s="25"/>
       <c r="AP26" s="26"/>
     </row>
-    <row r="27" spans="1:42">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D27" t="s">
         <v>44</v>
       </c>
@@ -3003,7 +3003,7 @@
       <c r="AO27" s="25"/>
       <c r="AP27" s="26"/>
     </row>
-    <row r="28" spans="1:42">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D28" t="s">
         <v>47</v>
       </c>
@@ -3047,7 +3047,7 @@
       <c r="AO28" s="25"/>
       <c r="AP28" s="26"/>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D29" t="s">
         <v>50</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="AO29" s="25"/>
       <c r="AP29" s="26"/>
     </row>
-    <row r="30" spans="1:42">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D30" t="s">
         <v>52</v>
       </c>
@@ -3135,7 +3135,7 @@
       <c r="AO30" s="25"/>
       <c r="AP30" s="26"/>
     </row>
-    <row r="31" spans="1:42">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D31" t="s">
         <v>55</v>
       </c>
@@ -3183,7 +3183,7 @@
       <c r="AO31" s="30"/>
       <c r="AP31" s="27"/>
     </row>
-    <row r="32" spans="1:42">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D32" t="s">
         <v>58</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="AA32" s="7"/>
       <c r="AB32" s="8"/>
     </row>
-    <row r="33" spans="1:40">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D33" t="s">
         <v>59</v>
       </c>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="AN33" s="63"/>
     </row>
-    <row r="34" spans="1:40">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D34" t="s">
         <v>60</v>
       </c>
@@ -3318,7 +3318,7 @@
       <c r="AM34" s="63"/>
       <c r="AN34" s="63"/>
     </row>
-    <row r="35" spans="1:40">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D35" t="s">
         <v>61</v>
       </c>
@@ -3363,7 +3363,7 @@
       <c r="AM35" s="63"/>
       <c r="AN35" s="63"/>
     </row>
-    <row r="36" spans="1:40">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D36" t="s">
         <v>62</v>
       </c>
@@ -3402,7 +3402,7 @@
       <c r="AK36" s="61"/>
       <c r="AL36" s="66"/>
     </row>
-    <row r="37" spans="1:40" ht="16.149999999999999" customHeight="1">
+    <row r="37" spans="1:40" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D37" t="s">
         <v>63</v>
       </c>
@@ -3445,7 +3445,7 @@
       <c r="AM37" s="31"/>
       <c r="AN37" s="32"/>
     </row>
-    <row r="38" spans="1:40">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D38" t="s">
         <v>64</v>
       </c>
@@ -3486,7 +3486,7 @@
       <c r="AM38" s="31"/>
       <c r="AN38" s="32"/>
     </row>
-    <row r="39" spans="1:40">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D39" t="s">
         <v>65</v>
       </c>
@@ -3527,7 +3527,7 @@
       <c r="AM39" s="31"/>
       <c r="AN39" s="32"/>
     </row>
-    <row r="40" spans="1:40">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="D40" s="1"/>
@@ -3564,7 +3564,7 @@
       <c r="AF40" s="61"/>
       <c r="AG40" s="62"/>
     </row>
-    <row r="41" spans="1:40">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A41" s="15" t="s">
         <v>32</v>
       </c>
@@ -3655,7 +3655,7 @@
       <c r="AF41" s="61"/>
       <c r="AG41" s="62"/>
     </row>
-    <row r="42" spans="1:40">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.4">
       <c r="A42" s="21" t="s">
         <v>52</v>
       </c>
@@ -3698,7 +3698,7 @@
       <c r="AF42" s="61"/>
       <c r="AG42" s="62"/>
     </row>
-    <row r="43" spans="1:40">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D43" t="s">
         <v>40</v>
       </c>
@@ -3735,7 +3735,7 @@
       <c r="AF43" s="61"/>
       <c r="AG43" s="62"/>
     </row>
-    <row r="44" spans="1:40">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D44" t="s">
         <v>42</v>
       </c>
@@ -3772,7 +3772,7 @@
       <c r="AF44" s="61"/>
       <c r="AG44" s="62"/>
     </row>
-    <row r="45" spans="1:40">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D45" t="s">
         <v>44</v>
       </c>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="AG45" s="62"/>
     </row>
-    <row r="46" spans="1:40">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D46" t="s">
         <v>47</v>
       </c>
@@ -3837,7 +3837,7 @@
       <c r="AF46" s="62"/>
       <c r="AG46" s="62"/>
     </row>
-    <row r="47" spans="1:40">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D47" t="s">
         <v>50</v>
       </c>
@@ -3868,7 +3868,7 @@
       <c r="AF47" s="62"/>
       <c r="AG47" s="62"/>
     </row>
-    <row r="48" spans="1:40">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.4">
       <c r="D48" t="s">
         <v>52</v>
       </c>
@@ -3899,7 +3899,7 @@
       <c r="AF48" s="62"/>
       <c r="AG48" s="62"/>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D49" t="s">
         <v>55</v>
       </c>
@@ -3930,7 +3930,7 @@
       <c r="AF49" s="62"/>
       <c r="AG49" s="62"/>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D50" t="s">
         <v>58</v>
       </c>
@@ -3961,7 +3961,7 @@
       <c r="AF50" s="62"/>
       <c r="AG50" s="62"/>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D51" t="s">
         <v>59</v>
       </c>
@@ -3990,7 +3990,7 @@
       <c r="AA51" s="7"/>
       <c r="AB51" s="8"/>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D52" t="s">
         <v>60</v>
       </c>
@@ -4019,7 +4019,7 @@
       <c r="AA52" s="7"/>
       <c r="AB52" s="8"/>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D53" t="s">
         <v>61</v>
       </c>
@@ -4048,7 +4048,7 @@
       <c r="AA53" s="7"/>
       <c r="AB53" s="8"/>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D54" t="s">
         <v>62</v>
       </c>
@@ -4077,7 +4077,7 @@
       <c r="AA54" s="7"/>
       <c r="AB54" s="8"/>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D55" t="s">
         <v>63</v>
       </c>
@@ -4106,7 +4106,7 @@
       <c r="AA55" s="7"/>
       <c r="AB55" s="8"/>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D56" t="s">
         <v>64</v>
       </c>
@@ -4135,7 +4135,7 @@
       <c r="AA56" s="7"/>
       <c r="AB56" s="8"/>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.4">
       <c r="D57" t="s">
         <v>65</v>
       </c>
@@ -4164,7 +4164,7 @@
       <c r="AA57" s="10"/>
       <c r="AB57" s="11"/>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="D58" s="1"/>
@@ -4235,9 +4235,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="3" spans="2:27">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B3" s="33" t="s">
         <v>37</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="Z3" s="69"/>
       <c r="AA3" s="34"/>
     </row>
-    <row r="4" spans="2:27">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B4" s="35"/>
       <c r="C4" s="36">
         <v>1</v>
@@ -4343,7 +4343,7 @@
       </c>
       <c r="AA4" s="35"/>
     </row>
-    <row r="5" spans="2:27">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B5" s="37" t="s">
         <v>38</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:27">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B6" s="37" t="s">
         <v>40</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:27" ht="18">
+    <row r="7" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B7" s="37" t="s">
         <v>42</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:27" ht="18">
+    <row r="8" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B8" s="37" t="s">
         <v>44</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:27" ht="18">
+    <row r="9" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B9" s="37" t="s">
         <v>47</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:27" ht="18">
+    <row r="10" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B10" s="37" t="s">
         <v>50</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:27" ht="18">
+    <row r="11" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B11" s="37" t="s">
         <v>52</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="2:27" ht="18">
+    <row r="12" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B12" s="37" t="s">
         <v>55</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:27">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B13" s="37" t="s">
         <v>58</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="2:27">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B14" s="43" t="s">
         <v>59</v>
       </c>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="AA14" s="35"/>
     </row>
-    <row r="15" spans="2:27">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B15" s="37" t="s">
         <v>60</v>
       </c>
@@ -4939,7 +4939,7 @@
       </c>
       <c r="AA15" s="34"/>
     </row>
-    <row r="16" spans="2:27">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B16" s="37" t="s">
         <v>61</v>
       </c>
@@ -4973,7 +4973,7 @@
       </c>
       <c r="AA16" s="34"/>
     </row>
-    <row r="17" spans="2:27">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B17" s="37" t="s">
         <v>62</v>
       </c>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="AA17" s="34"/>
     </row>
-    <row r="18" spans="2:27">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B18" s="37" t="s">
         <v>63</v>
       </c>
@@ -5041,7 +5041,7 @@
       </c>
       <c r="AA18" s="34"/>
     </row>
-    <row r="19" spans="2:27">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B19" s="37" t="s">
         <v>64</v>
       </c>
@@ -5119,7 +5119,7 @@
       </c>
       <c r="AA19" s="34"/>
     </row>
-    <row r="20" spans="2:27">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B20" s="34"/>
       <c r="C20" s="36">
         <v>1</v>
@@ -5195,7 +5195,7 @@
       </c>
       <c r="AA20" s="34"/>
     </row>
-    <row r="21" spans="2:27">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
@@ -5227,7 +5227,7 @@
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
     </row>
-    <row r="22" spans="2:27" ht="16.149999999999999" thickBot="1">
+    <row r="22" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -5259,7 +5259,7 @@
       <c r="Z22" s="34"/>
       <c r="AA22" s="34"/>
     </row>
-    <row r="23" spans="2:27">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.4">
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
@@ -5291,7 +5291,7 @@
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
     </row>
-    <row r="24" spans="2:27" ht="16.149999999999999" thickBot="1">
+    <row r="24" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
@@ -5350,6 +5350,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009892A9DD32002F4F826D12D9986E78B0" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="117611f314cda0a79d2af28b54ae3898">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc74464e-86fe-482d-93f3-1ffecc162557" xmlns:ns3="676739f8-ea59-4bde-a77e-78e2df6ab591" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ec0ad223d59dd7c7c3f5c0582522d2a" ns2:_="" ns3:_="">
     <xsd:import namespace="bc74464e-86fe-482d-93f3-1ffecc162557"/>
@@ -5590,23 +5599,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5035CA6-1FDB-41A8-8F2D-A2829E9EB9BB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5035CA6-1FDB-41A8-8F2D-A2829E9EB9BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bc74464e-86fe-482d-93f3-1ffecc162557"/>
+    <ds:schemaRef ds:uri="676739f8-ea59-4bde-a77e-78e2df6ab591"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{420EF5BF-E933-489E-9EED-235AA6CD4230}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{514A0F8E-E43D-426F-9FC6-493D23D23525}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{514A0F8E-E43D-426F-9FC6-493D23D23525}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{420EF5BF-E933-489E-9EED-235AA6CD4230}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bc74464e-86fe-482d-93f3-1ffecc162557"/>
+    <ds:schemaRef ds:uri="676739f8-ea59-4bde-a77e-78e2df6ab591"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>